<commit_message>
updating to read data from Pepperwood master, and adding June 2022 data
</commit_message>
<xml_diff>
--- a/results/sampletable.xlsx
+++ b/results/sampletable.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/PepperwoodLFM/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Google Drive/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/PepperwoodLFM/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{95868718-4D6D-A241-B44D-2082FE6456E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC04334-A13D-7648-A374-378880F29B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="840" yWindow="560" windowWidth="27960" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sampletable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -229,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1079,7 +1090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1089,7 +1100,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="5.5" customWidth="1"/>
     <col min="5" max="5" width="3.6640625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
combining data, outputing summary tables, etc.
</commit_message>
<xml_diff>
--- a/results/sampletable.xlsx
+++ b/results/sampletable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Google Drive/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/PepperwoodLFM/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/PepperwoodLFM/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC04334-A13D-7648-A374-378880F29B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA62A00-8944-8C4D-B833-835133E0044D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="560" windowWidth="27960" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t>BG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>BOH</t>
   </si>
@@ -63,9 +60,6 @@
     <t>ARBMEN</t>
   </si>
   <si>
-    <t>BACPIL</t>
-  </si>
-  <si>
     <t>CEACUN</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Sp2</t>
   </si>
   <si>
-    <t>Sites</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>Am</t>
   </si>
   <si>
-    <t>Bp</t>
-  </si>
-  <si>
     <t>Cc</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>Arbutus mensiezii</t>
   </si>
   <si>
-    <t>Baccharis pilularis</t>
-  </si>
-  <si>
     <t>Ceanothus cuneatus</t>
   </si>
   <si>
@@ -195,9 +180,6 @@
     <t>Madrone</t>
   </si>
   <si>
-    <t>Coyotebush</t>
-  </si>
-  <si>
     <t>Buckbrush</t>
   </si>
   <si>
@@ -235,6 +217,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>6*</t>
+  </si>
+  <si>
+    <t>* Only three individuals sampled in June 2022</t>
   </si>
 </sst>
 </file>
@@ -730,11 +718,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1094,7 +1082,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,20 +1091,19 @@
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="5.5" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1124,29 +1111,26 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -1170,595 +1154,517 @@
         <v>6</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>6</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <f>SUM(E4:L4)</f>
+        <f>SUM(E4:K4)</f>
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
+        <v>23</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
       </c>
       <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
-        <f t="shared" ref="M5:M16" si="0">SUM(E5:L5)</f>
+        <f>SUM(E5:K5)</f>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E6:K6)</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E8:K8)</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E9:K9)</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
       </c>
       <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E10:K10)</f>
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>2</v>
       </c>
-      <c r="J11" s="3">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
       <c r="L11" s="3">
-        <v>2</v>
-      </c>
-      <c r="M11" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E11:K11)</f>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>4</v>
-      </c>
-      <c r="K12" s="3">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" s="3">
-        <v>2</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E12:K12)</f>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
       </c>
       <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E13:K13)</f>
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
+        <v>32</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0</v>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
       </c>
       <c r="L14" s="3">
-        <v>2</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E14:K14)</f>
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
       </c>
       <c r="L15" s="3">
-        <v>4</v>
-      </c>
-      <c r="M15" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E15:K15)</f>
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="3">
+        <f>SUM(E4:E15)</f>
+        <v>11</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ref="E16:K16" si="0">SUM(F4:F15)</f>
+        <v>4</v>
+      </c>
+      <c r="G16" s="3">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L16" s="3">
+        <f>SUM(E16:K16)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>4</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1</v>
-      </c>
-      <c r="M16" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="4">
-        <f>SUM(E4:E16)</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" ref="F17:L17" si="1">SUM(F4:F16)</f>
-        <v>11</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="K17" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="M17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>